<commit_message>
dev-1.0.0 : update template labor new
</commit_message>
<xml_diff>
--- a/public/files/Template_Labor.xlsx
+++ b/public/files/Template_Labor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\#AIIA\2022\Trial SYSTEM BUDGET\Trial 31-10\New template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neli\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -74,15 +74,6 @@
     <t>MAR</t>
   </si>
   <si>
-    <t>FY 2022 1st</t>
-  </si>
-  <si>
-    <t>FY 2022 2nd</t>
-  </si>
-  <si>
-    <t>FY 2022 TOTAL</t>
-  </si>
-  <si>
     <t>5212110101</t>
   </si>
   <si>
@@ -789,6 +780,15 @@
   </si>
   <si>
     <t>SGA0048</t>
+  </si>
+  <si>
+    <t>FY 2023 1st</t>
+  </si>
+  <si>
+    <t>FY 2023 2nd</t>
+  </si>
+  <si>
+    <t>FY 2023 TOTAL</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1191,7 @@
   <dimension ref="A1:S218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1254,27 +1254,27 @@
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>16</v>
+        <v>252</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>17</v>
+        <v>253</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -1303,16 +1303,16 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -1341,16 +1341,16 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -1379,16 +1379,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -1417,16 +1417,16 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -1455,16 +1455,16 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -1493,16 +1493,16 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -1531,16 +1531,16 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -1569,16 +1569,16 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1607,16 +1607,16 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1645,16 +1645,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -1683,16 +1683,16 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -1721,16 +1721,16 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -1759,16 +1759,16 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -1797,16 +1797,16 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -1835,16 +1835,16 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -1873,16 +1873,16 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -1911,16 +1911,16 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1949,16 +1949,16 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1987,16 +1987,16 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -2025,16 +2025,16 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -2063,16 +2063,16 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -2101,16 +2101,16 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -2139,16 +2139,16 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -2177,16 +2177,16 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -2215,16 +2215,16 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -2253,16 +2253,16 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -2291,16 +2291,16 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -2329,16 +2329,16 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -2367,16 +2367,16 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -2405,16 +2405,16 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -2443,16 +2443,16 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2481,16 +2481,16 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2519,16 +2519,16 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2557,16 +2557,16 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2595,16 +2595,16 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2633,16 +2633,16 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2671,16 +2671,16 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -2709,16 +2709,16 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
@@ -2747,16 +2747,16 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -2785,16 +2785,16 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
@@ -2823,16 +2823,16 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
@@ -2861,16 +2861,16 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
@@ -2899,16 +2899,16 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
@@ -2937,16 +2937,16 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -2975,16 +2975,16 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
@@ -3013,16 +3013,16 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
@@ -3051,16 +3051,16 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
@@ -3089,16 +3089,16 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
@@ -3127,16 +3127,16 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C51" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -3165,16 +3165,16 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
@@ -3203,16 +3203,16 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
@@ -3241,16 +3241,16 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
@@ -3279,16 +3279,16 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
@@ -3317,16 +3317,16 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
@@ -3355,16 +3355,16 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
@@ -3393,16 +3393,16 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
@@ -3431,16 +3431,16 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
@@ -3469,16 +3469,16 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
@@ -3507,16 +3507,16 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
@@ -3545,16 +3545,16 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
@@ -3583,16 +3583,16 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
@@ -3621,16 +3621,16 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
@@ -3659,16 +3659,16 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
@@ -3697,16 +3697,16 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
@@ -3735,16 +3735,16 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
@@ -3773,16 +3773,16 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
@@ -3811,16 +3811,16 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
@@ -3849,16 +3849,16 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A70" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
@@ -3887,16 +3887,16 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
@@ -3925,16 +3925,16 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
@@ -3963,16 +3963,16 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
@@ -4001,16 +4001,16 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
@@ -4039,16 +4039,16 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A75" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
@@ -4077,16 +4077,16 @@
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
@@ -4115,16 +4115,16 @@
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
@@ -4153,16 +4153,16 @@
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
@@ -4191,16 +4191,16 @@
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
@@ -4229,16 +4229,16 @@
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A80" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
@@ -4267,16 +4267,16 @@
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A81" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
@@ -4305,16 +4305,16 @@
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A82" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
@@ -4343,16 +4343,16 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A83" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
@@ -4381,16 +4381,16 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A84" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
@@ -4419,16 +4419,16 @@
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A85" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
@@ -4457,16 +4457,16 @@
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A86" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
@@ -4495,16 +4495,16 @@
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A87" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
@@ -4533,16 +4533,16 @@
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A88" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
@@ -4571,16 +4571,16 @@
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A89" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
@@ -4609,16 +4609,16 @@
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A90" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
@@ -4647,16 +4647,16 @@
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A91" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
@@ -4685,16 +4685,16 @@
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A92" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E92" s="7"/>
       <c r="F92" s="7"/>
@@ -4723,16 +4723,16 @@
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A93" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
@@ -4761,16 +4761,16 @@
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A94" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
@@ -4799,16 +4799,16 @@
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A95" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
@@ -4837,16 +4837,16 @@
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A96" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
@@ -4875,16 +4875,16 @@
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A97" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
@@ -4913,16 +4913,16 @@
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A98" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C98" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D98" s="6" t="s">
         <v>208</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
@@ -4951,16 +4951,16 @@
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A99" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
@@ -4989,16 +4989,16 @@
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A100" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
@@ -5027,16 +5027,16 @@
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A101" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
@@ -5065,16 +5065,16 @@
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A102" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
@@ -5103,16 +5103,16 @@
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A103" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E103" s="7"/>
       <c r="F103" s="7"/>
@@ -5141,16 +5141,16 @@
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A104" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E104" s="7"/>
       <c r="F104" s="7"/>
@@ -5179,16 +5179,16 @@
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A105" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E105" s="7"/>
       <c r="F105" s="7"/>
@@ -5217,16 +5217,16 @@
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A106" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E106" s="7"/>
       <c r="F106" s="7"/>
@@ -5255,16 +5255,16 @@
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A107" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E107" s="7"/>
       <c r="F107" s="7"/>
@@ -5293,16 +5293,16 @@
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A108" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E108" s="7"/>
       <c r="F108" s="7"/>
@@ -5331,16 +5331,16 @@
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A109" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
@@ -5369,16 +5369,16 @@
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A110" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E110" s="7"/>
       <c r="F110" s="7"/>
@@ -5407,16 +5407,16 @@
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
@@ -5445,16 +5445,16 @@
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A112" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E112" s="7"/>
       <c r="F112" s="7"/>
@@ -5483,16 +5483,16 @@
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A113" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E113" s="7"/>
       <c r="F113" s="7"/>
@@ -5521,16 +5521,16 @@
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A114" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E114" s="7"/>
       <c r="F114" s="7"/>
@@ -5559,16 +5559,16 @@
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A115" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E115" s="7"/>
       <c r="F115" s="7"/>
@@ -5597,16 +5597,16 @@
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E116" s="7"/>
       <c r="F116" s="7"/>
@@ -5635,16 +5635,16 @@
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A117" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E117" s="7"/>
       <c r="F117" s="7"/>
@@ -5673,16 +5673,16 @@
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E118" s="7"/>
       <c r="F118" s="7"/>
@@ -5711,16 +5711,16 @@
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A119" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E119" s="7"/>
       <c r="F119" s="7"/>
@@ -5749,16 +5749,16 @@
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A120" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E120" s="7"/>
       <c r="F120" s="7"/>
@@ -5787,16 +5787,16 @@
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A121" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E121" s="7"/>
       <c r="F121" s="7"/>
@@ -5825,16 +5825,16 @@
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A122" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E122" s="7"/>
       <c r="F122" s="7"/>
@@ -5863,16 +5863,16 @@
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A123" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E123" s="7"/>
       <c r="F123" s="7"/>
@@ -5901,16 +5901,16 @@
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A124" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E124" s="7"/>
       <c r="F124" s="7"/>
@@ -5939,16 +5939,16 @@
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A125" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
@@ -5977,16 +5977,16 @@
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A126" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E126" s="7"/>
       <c r="F126" s="7"/>
@@ -6015,16 +6015,16 @@
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A127" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E127" s="7"/>
       <c r="F127" s="7"/>
@@ -6053,16 +6053,16 @@
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A128" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E128" s="7"/>
       <c r="F128" s="7"/>
@@ -6091,16 +6091,16 @@
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A129" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E129" s="7"/>
       <c r="F129" s="7"/>
@@ -6129,16 +6129,16 @@
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A130" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E130" s="7"/>
       <c r="F130" s="7"/>
@@ -6167,16 +6167,16 @@
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A131" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E131" s="7"/>
       <c r="F131" s="7"/>
@@ -6205,16 +6205,16 @@
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A132" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E132" s="7"/>
       <c r="F132" s="7"/>
@@ -6243,16 +6243,16 @@
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A133" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E133" s="7"/>
       <c r="F133" s="7"/>
@@ -6281,16 +6281,16 @@
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A134" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E134" s="7"/>
       <c r="F134" s="7"/>
@@ -6319,16 +6319,16 @@
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A135" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E135" s="7"/>
       <c r="F135" s="7"/>
@@ -6357,16 +6357,16 @@
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A136" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E136" s="7"/>
       <c r="F136" s="7"/>
@@ -6395,16 +6395,16 @@
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A137" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E137" s="7"/>
       <c r="F137" s="7"/>
@@ -6433,16 +6433,16 @@
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A138" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E138" s="7"/>
       <c r="F138" s="7"/>
@@ -6471,16 +6471,16 @@
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A139" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E139" s="7"/>
       <c r="F139" s="7"/>
@@ -6509,16 +6509,16 @@
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A140" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E140" s="7"/>
       <c r="F140" s="7"/>
@@ -6547,16 +6547,16 @@
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A141" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E141" s="7"/>
       <c r="F141" s="7"/>
@@ -6585,16 +6585,16 @@
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A142" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E142" s="7"/>
       <c r="F142" s="7"/>
@@ -7762,7 +7762,7 @@
       <c r="Q218" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="CU7OLWepWvdH72Jst0vyEgY9+/SsIvH9atH+XAdSdwoGTViS8Plbx4f6KhuA+b/vCb69xbvCrGxdDkgDfY8fqQ==" saltValue="eTeZep0rbOqzVtArqEwAUQ==" spinCount="100000" sheet="1" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <protectedRanges>
     <protectedRange sqref="E1:P1048576" name="OPEN 1"/>
     <protectedRange sqref="A143:XFD187" name="OPEN 2"/>

</xml_diff>